<commit_message>
Description de la mise à jour
</commit_message>
<xml_diff>
--- a/docs/Tableau de synthèse - Epreuve E4 - BTS SIO 2023.xlsx
+++ b/docs/Tableau de synthèse - Epreuve E4 - BTS SIO 2023.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtr\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtr\Desktop\bts sio 1A\SLAM\portfolio\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D7F4C6-EBB4-4E1E-9CEB-CC341A992B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82CEDC5-B2FA-4D7D-9C9E-94404A7C845C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,10 +16,13 @@
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$31</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$32</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -122,22 +125,25 @@
 </t>
   </si>
   <si>
-    <t>Du 06/02/2023 au 10/02/2023</t>
+    <t>Installation et Configuration d'un serveur GLPI pour la gestion des tickets  d'incidents</t>
   </si>
   <si>
-    <t>Du 26/10/2022 au 13/01/2023</t>
+    <t xml:space="preserve">Création d'une entreprise fictive (ACE) </t>
   </si>
   <si>
-    <t>Du 03/23 au 05/23</t>
+    <t xml:space="preserve">Organisation d'une solution technique (M2L) </t>
   </si>
   <si>
-    <t>Du 11/22 à maintenant</t>
+    <t>Gestion de son réseau professionnel (Linkedin)</t>
   </si>
   <si>
-    <t>Du 02/23 au 03/23</t>
+    <t>Gestion d'une librairie virtuelle (API Google Book)</t>
   </si>
   <si>
-    <t>Du 04/23 à maintenant</t>
+    <t>Mise en place d'un flux RSS (Feedly)</t>
+  </si>
+  <si>
+    <t>18/09 à maintenant</t>
   </si>
   <si>
     <t>Réalisations en milieu professionnel en cours de première année</t>
@@ -146,34 +152,52 @@
     <t>Réalisations en milieu professionnel en cours de seconde année</t>
   </si>
   <si>
-    <t>NOM et prénom : Marion TRINH</t>
+    <t>Réalisation d'un site internet en HTML, CSS et Javascript</t>
+  </si>
+  <si>
+    <t>Réalisation d'une application en VueJs</t>
+  </si>
+  <si>
+    <t>NOM et prénom : TRINH Marion</t>
   </si>
   <si>
     <t>Adresse URL du portfolio : https://nnarion.github.io/portfolio/</t>
   </si>
   <si>
-    <t>Mise en place d'un flux RSS (Feedly)</t>
+    <t>18/09/23 au 18/09/23</t>
   </si>
   <si>
-    <t>Création d'une librairie virtuelle (API Google Book)</t>
+    <t>Du 01/03/23 au 01/05/23</t>
   </si>
   <si>
-    <t>Gestion de son réseau professionnel (Linkedin)</t>
+    <t>Du 06/02/23 au 10/02/23</t>
   </si>
   <si>
-    <t>Mise en place d'un environnement de travail personnel</t>
+    <t>Du 10/02/23 au 10/03/23</t>
   </si>
   <si>
-    <t>Organisation d'une solution technique (M2L)</t>
+    <t>Du 01/04/23 à maintenant</t>
   </si>
   <si>
-    <t>Création d'une entreprise fictive (Ace)</t>
+    <t>Du 01/06/23 au 01/07/23</t>
   </si>
   <si>
-    <t>Réalisation d'une application en VueJs</t>
+    <t>Création d'une solution lourde pour M2L</t>
   </si>
   <si>
-    <t>Réalisation d'un site internet en HTML, CSS et Javascript</t>
+    <t>Création d'une solution légère pour M2L</t>
+  </si>
+  <si>
+    <t>Du 26/10/23 au 13/01/23</t>
+  </si>
+  <si>
+    <t>Du 05/11/23 à maintenant</t>
+  </si>
+  <si>
+    <t>Inventaire des équipements réseaux</t>
+  </si>
+  <si>
+    <t>Du 18/09/23 au 18/09/23</t>
   </si>
 </sst>
 </file>
@@ -183,7 +207,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -240,11 +264,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="16"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -684,9 +703,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -776,6 +792,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Euro" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1271,13 +1290,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>19879</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>6626</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1324,13 +1343,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>19879</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>6626</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1342,218 +1361,6 @@
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
               <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{12906C3A-69F6-4731-AB27-2B37BE447A13}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="11696700" y="10610850"/>
-          <a:ext cx="1267654" cy="511451"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>19879</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>536713</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="30" name="Connecteur droit 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07466A58-37A8-46D2-892C-089ECD8333A8}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{46B63E76-B3E1-4727-93C3-87EC0FDF22E6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11696700" y="10610850"/>
-          <a:ext cx="1267654" cy="508138"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>19879</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>6626</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="31" name="Connecteur droit 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F21E08C0-AFEF-4F59-8E2B-48A0E75703D4}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{07466A58-37A8-46D2-892C-089ECD8333A8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="11696700" y="10610850"/>
-          <a:ext cx="1267654" cy="511451"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>19879</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>536713</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="32" name="Connecteur droit 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CB700BC-6AED-4157-9972-9A726AE2DAEE}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{F21E08C0-AFEF-4F59-8E2B-48A0E75703D4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11696700" y="10610850"/>
-          <a:ext cx="1267654" cy="508138"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>19879</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>6626</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="33" name="Connecteur droit 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E3E6C1C-9A71-4318-B65D-14DBC8241169}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{9CB700BC-6AED-4157-9972-9A726AE2DAEE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1600,13 +1407,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="34" name="Connecteur droit 5">
+        <xdr:cNvPr id="30" name="Connecteur droit 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA680B88-F0B7-4CC2-B6E5-22E927B0F96A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07466A58-37A8-46D2-892C-089ECD8333A8}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{9E3E6C1C-9A71-4318-B65D-14DBC8241169}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{46B63E76-B3E1-4727-93C3-87EC0FDF22E6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1649,6 +1456,218 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>19879</xdr:colOff>
       <xdr:row>19</xdr:row>
+      <xdr:rowOff>6626</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F21E08C0-AFEF-4F59-8E2B-48A0E75703D4}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{07466A58-37A8-46D2-892C-089ECD8333A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11696700" y="10610850"/>
+          <a:ext cx="1267654" cy="511451"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>536713</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="Connecteur droit 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CB700BC-6AED-4157-9972-9A726AE2DAEE}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{F21E08C0-AFEF-4F59-8E2B-48A0E75703D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11696700" y="10610850"/>
+          <a:ext cx="1267654" cy="508138"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>6626</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E3E6C1C-9A71-4318-B65D-14DBC8241169}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{9CB700BC-6AED-4157-9972-9A726AE2DAEE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11696700" y="10610850"/>
+          <a:ext cx="1267654" cy="511451"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>536713</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Connecteur droit 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA680B88-F0B7-4CC2-B6E5-22E927B0F96A}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{9E3E6C1C-9A71-4318-B65D-14DBC8241169}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11696700" y="10610850"/>
+          <a:ext cx="1267654" cy="508138"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>6626</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1708,7 +1727,7 @@
       <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="38" name="Ink 37">
+            <xdr14:cNvPr id="38" name="Encre 37">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                   <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D3EB70A-8F7A-419E-BC0C-04972A8E0A82}"/>
@@ -1779,7 +1798,7 @@
       <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="39" name="Ink 38">
+            <xdr14:cNvPr id="39" name="Encre 38">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                   <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A1A1316-E05F-4D65-B95A-EB29DB623A51}"/>
@@ -2108,7 +2127,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>19879</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>6626</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2129,6 +2148,2279 @@
         <a:xfrm flipV="1">
           <a:off x="7953375" y="8029575"/>
           <a:ext cx="1267654" cy="568601"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>6626</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{847E3138-D932-45DC-8624-C2DD2CAB5CA1}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{FA680B88-F0B7-4CC2-B6E5-22E927B0F96A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7029174" y="11148391"/>
+          <a:ext cx="1328531" cy="514626"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>504963</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Connecteur droit 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82CC63FF-9ED2-4069-9405-859C435DC27A}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{9E3E6C1C-9A71-4318-B65D-14DBC8241169}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7029174" y="11148391"/>
+          <a:ext cx="1328531" cy="504963"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>6626</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{679B92B3-0F82-419B-89B0-BFD4CCA83330}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{82CC63FF-9ED2-4069-9405-859C435DC27A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6705600" y="11115675"/>
+          <a:ext cx="1267654" cy="511451"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>504963</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="Connecteur droit 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A08700E-A663-4DD7-A05B-3C2EB40E5F72}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{679B92B3-0F82-419B-89B0-BFD4CCA83330}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6705600" y="11115675"/>
+          <a:ext cx="1267654" cy="504963"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>6626</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52A0ABAF-E0B6-47EC-A396-EA76B430873B}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{9A08700E-A663-4DD7-A05B-3C2EB40E5F72}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6705600" y="11115675"/>
+          <a:ext cx="1267654" cy="511451"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>504963</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="Connecteur droit 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54B4528C-A2E2-486C-BFDD-F312F4A85ECC}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{52A0ABAF-E0B6-47EC-A396-EA76B430873B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6705600" y="11115675"/>
+          <a:ext cx="1267654" cy="504963"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>6626</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97206F0B-04CC-48F1-96BD-AD4C1F9FBF9B}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{54B4528C-A2E2-486C-BFDD-F312F4A85ECC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9201150" y="11620500"/>
+          <a:ext cx="1267654" cy="511451"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>504963</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Connecteur droit 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7A365D7-82E1-4CF5-B167-5ACE9DD2F22F}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{97206F0B-04CC-48F1-96BD-AD4C1F9FBF9B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9201150" y="11620500"/>
+          <a:ext cx="1267654" cy="504963"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>6626</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7686A4F7-283F-40A3-8B2C-D8FDA1E34436}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{E7A365D7-82E1-4CF5-B167-5ACE9DD2F22F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9201150" y="11620500"/>
+          <a:ext cx="1267654" cy="511451"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>504963</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="40" name="Connecteur droit 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D28A03C-109B-4AC8-A195-557A99460E85}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{7686A4F7-283F-40A3-8B2C-D8FDA1E34436}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9201150" y="11620500"/>
+          <a:ext cx="1267654" cy="504963"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>6626</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="59" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51176E10-C4C2-41C0-B078-59B2B4E72B61}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{93723703-4CF6-4B24-BAA6-818A95244B8E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12276667" y="12403667"/>
+          <a:ext cx="1332212" cy="6626"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>6626</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="60" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBDFCBFF-8B99-444A-A797-CF0D5D254CD1}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{12906C3A-69F6-4731-AB27-2B37BE447A13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10964333" y="12403667"/>
+          <a:ext cx="1332213" cy="6626"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>536713</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="61" name="Connecteur droit 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0C7A3FF-8C9A-465F-9E16-E5A0496265E2}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{46B63E76-B3E1-4727-93C3-87EC0FDF22E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12276667" y="12403667"/>
+          <a:ext cx="1332212" cy="504963"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>6626</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="62" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33B31566-50E3-4D2A-99FA-A1A09FB5ADDE}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{07466A58-37A8-46D2-892C-089ECD8333A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12276667" y="12403667"/>
+          <a:ext cx="1332212" cy="514626"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>536713</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="63" name="Connecteur droit 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{206FA8AE-34C8-4FC7-9FDB-07134FA6567B}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{F21E08C0-AFEF-4F59-8E2B-48A0E75703D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12276667" y="12403667"/>
+          <a:ext cx="1332212" cy="504963"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>6626</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="64" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A24EED1A-6759-4E3E-9E8E-1A7E3389800E}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{9CB700BC-6AED-4157-9972-9A726AE2DAEE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12276667" y="12403667"/>
+          <a:ext cx="1332212" cy="514626"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>6626</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="65" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A17D9ED-3433-449B-B02F-4DB0F88AB50E}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{93723703-4CF6-4B24-BAA6-818A95244B8E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12276667" y="12403667"/>
+          <a:ext cx="1332212" cy="6626"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>6626</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="66" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1A0D99D-BD99-4BAF-AC0A-2E0627ABABC6}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{12906C3A-69F6-4731-AB27-2B37BE447A13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10964333" y="12403667"/>
+          <a:ext cx="1332213" cy="6626"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>536713</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="67" name="Connecteur droit 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D6F6B22-28FA-4ADF-B887-A88AF4C4AFC2}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{46B63E76-B3E1-4727-93C3-87EC0FDF22E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12276667" y="12403667"/>
+          <a:ext cx="1332212" cy="504963"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>6626</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="68" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F36E6FE8-4339-4C84-9D51-FB104CAC9F33}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{07466A58-37A8-46D2-892C-089ECD8333A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12276667" y="12403667"/>
+          <a:ext cx="1332212" cy="514626"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>536713</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="69" name="Connecteur droit 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA703AC1-20C9-4FEF-B964-01D2618E62D5}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{F21E08C0-AFEF-4F59-8E2B-48A0E75703D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12276667" y="12403667"/>
+          <a:ext cx="1332212" cy="504963"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>6626</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="70" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{898A0982-C59D-4960-92A0-CE1A97149A09}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{9CB700BC-6AED-4157-9972-9A726AE2DAEE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12276667" y="12403667"/>
+          <a:ext cx="1332212" cy="514626"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>6626</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="71" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFB68C0C-F14B-49B3-887B-61DBF3B0A05F}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{93723703-4CF6-4B24-BAA6-818A95244B8E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12276667" y="12403667"/>
+          <a:ext cx="1332212" cy="6626"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>6626</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="72" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F75F8544-C61B-4F47-AF32-803A465A2E15}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{12906C3A-69F6-4731-AB27-2B37BE447A13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10964333" y="12403667"/>
+          <a:ext cx="1332213" cy="6626"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>536713</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="73" name="Connecteur droit 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AF75789-8895-407E-BF58-1DAA0DDDFC91}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{46B63E76-B3E1-4727-93C3-87EC0FDF22E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12276667" y="12403667"/>
+          <a:ext cx="1332212" cy="504963"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>6626</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="74" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05DB1B92-FE23-4D9D-9C32-A19B74062A55}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{07466A58-37A8-46D2-892C-089ECD8333A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12276667" y="12403667"/>
+          <a:ext cx="1332212" cy="514626"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>536713</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="75" name="Connecteur droit 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3898326-A36B-43CE-B7B6-09ED7FA5854B}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{F21E08C0-AFEF-4F59-8E2B-48A0E75703D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12276667" y="12403667"/>
+          <a:ext cx="1332212" cy="504963"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>6626</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="76" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CB19D58-5FE4-4D73-8119-655CA60A4BDB}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{9CB700BC-6AED-4157-9972-9A726AE2DAEE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12276667" y="12403667"/>
+          <a:ext cx="1332212" cy="514626"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>6626</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="82" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73BA700E-1B2C-4D73-95C4-DAAD9A143612}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{93723703-4CF6-4B24-BAA6-818A95244B8E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12276667" y="12403667"/>
+          <a:ext cx="1332212" cy="6626"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>6626</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="83" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BB4040B-60D9-4129-BC2C-9207D3FF4CF3}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{12906C3A-69F6-4731-AB27-2B37BE447A13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10964333" y="12403667"/>
+          <a:ext cx="1332213" cy="6626"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>536713</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="84" name="Connecteur droit 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD3E9DA4-F5F1-48DE-B5F0-1A868E88840F}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{46B63E76-B3E1-4727-93C3-87EC0FDF22E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12276667" y="12403667"/>
+          <a:ext cx="1332212" cy="504963"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>6626</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="85" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6ACEA853-26B3-4229-A7FC-DA03D75F1503}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{07466A58-37A8-46D2-892C-089ECD8333A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12276667" y="12403667"/>
+          <a:ext cx="1332212" cy="514626"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>536713</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="86" name="Connecteur droit 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BF63993-1639-4737-BC1C-D6CC39A4648D}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{F21E08C0-AFEF-4F59-8E2B-48A0E75703D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12276667" y="12403667"/>
+          <a:ext cx="1332212" cy="504963"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>6626</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="87" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D8D1E68-7361-42B3-AB71-DEE391341F54}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{9CB700BC-6AED-4157-9972-9A726AE2DAEE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12276667" y="12403667"/>
+          <a:ext cx="1332212" cy="514626"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>6626</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="88" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4CAF6DA-3713-44BF-BA8C-EF6991B57862}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{93723703-4CF6-4B24-BAA6-818A95244B8E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10964333" y="12403667"/>
+          <a:ext cx="1332213" cy="6626"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>536713</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="89" name="Connecteur droit 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89D99B4E-5CD9-41C4-BD1A-B8CFA5AFF320}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{46B63E76-B3E1-4727-93C3-87EC0FDF22E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10964333" y="12403667"/>
+          <a:ext cx="1332213" cy="504963"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>6626</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="90" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38C3FF23-B119-425F-9908-BD9AAA38DA72}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{07466A58-37A8-46D2-892C-089ECD8333A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10964333" y="12403667"/>
+          <a:ext cx="1332213" cy="514626"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>536713</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="91" name="Connecteur droit 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65BA75F4-C583-453E-9BB0-91701AD39A15}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{F21E08C0-AFEF-4F59-8E2B-48A0E75703D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10964333" y="12403667"/>
+          <a:ext cx="1332213" cy="504963"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>6626</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="92" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CFC747E-86F7-40C4-9EC8-4E93429BBAF2}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{9CB700BC-6AED-4157-9972-9A726AE2DAEE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10964333" y="12403667"/>
+          <a:ext cx="1332213" cy="514626"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>536713</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="81" name="Connecteur droit 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2237F6FD-8622-476E-8BF8-0936A3CE229B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12276667" y="8057444"/>
+          <a:ext cx="1332212" cy="536713"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>6626</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="93" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19C66849-DD7C-4785-A6A3-AE20345AF980}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12276667" y="8057444"/>
+          <a:ext cx="1332212" cy="571071"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>6626</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="94" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D4277A2-0392-4B33-A06D-8813CCC451B9}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{E7A365D7-82E1-4CF5-B167-5ACE9DD2F22F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10964333" y="8057444"/>
+          <a:ext cx="1332213" cy="571071"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>504963</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="95" name="Connecteur droit 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA49FDBA-66F6-41F2-BE29-71E587A0F452}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{7686A4F7-283F-40A3-8B2C-D8FDA1E34436}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10964333" y="8057444"/>
+          <a:ext cx="1332213" cy="504963"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2540,10 +4832,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AQ77"/>
+  <dimension ref="A1:AQ78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="49" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="45" zoomScaleNormal="45" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2556,83 +4848,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="24"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:43" ht="41.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
-        <v>31</v>
+      <c r="A3" s="35" t="s">
+        <v>34</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="42" t="s">
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="43"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="42"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="41"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="40"/>
       <c r="F4" s="12" t="s">
         <v>5</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="18" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="33" t="s">
-        <v>32</v>
+      <c r="A5" s="32" t="s">
+        <v>35</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="35"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="34"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="30" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -2655,24 +4947,24 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="325" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="23"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="20" t="s">
+      <c r="A7" s="22"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="20" t="s">
         <v>21</v>
       </c>
       <c r="I7"/>
@@ -2712,16 +5004,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="27"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="26"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -2760,17 +5052,17 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="C9" s="14"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="16"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="15"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
@@ -2809,17 +5101,17 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="16"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="15"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
@@ -2858,17 +5150,17 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="16"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="15"/>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
@@ -2907,17 +5199,17 @@
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -2956,17 +5248,17 @@
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -3005,17 +5297,17 @@
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -3053,14 +5345,18 @@
       <c r="AQ14"/>
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="16"/>
+      <c r="A15" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="43"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -3098,14 +5394,18 @@
       <c r="AQ15"/>
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="16"/>
+      <c r="A16" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="15"/>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -3142,17 +5442,19 @@
       <c r="AP16"/>
       <c r="AQ16"/>
     </row>
-    <row r="17" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
+    <row r="17" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="30"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="15"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -3189,17 +5491,17 @@
       <c r="AP17"/>
       <c r="AQ17"/>
     </row>
-    <row r="18" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>40</v>
+    <row r="18" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A18" s="27" t="s">
+        <v>30</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="16"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="29"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -3238,15 +5540,17 @@
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="16"/>
+      <c r="B19" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="15"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -3284,14 +5588,18 @@
       <c r="AQ19"/>
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="16"/>
+      <c r="A20" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="15"/>
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20"/>
@@ -3331,12 +5639,12 @@
     <row r="21" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="8"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="16"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="15"/>
       <c r="I21"/>
       <c r="J21"/>
       <c r="K21"/>
@@ -3376,12 +5684,12 @@
     <row r="22" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="B22" s="8"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="16"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="15"/>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
@@ -3418,17 +5726,15 @@
       <c r="AP22"/>
       <c r="AQ22"/>
     </row>
-    <row r="23" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="30"/>
+    <row r="23" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="15"/>
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
@@ -3465,15 +5771,17 @@
       <c r="AP23"/>
       <c r="AQ23"/>
     </row>
-    <row r="24" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="16"/>
+    <row r="24" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A24" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="29"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -3513,12 +5821,12 @@
     <row r="25" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="B25" s="8"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="16"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="15"/>
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
@@ -3558,12 +5866,12 @@
     <row r="26" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="8"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="16"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="15"/>
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
@@ -3603,12 +5911,12 @@
     <row r="27" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="8"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="16"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="15"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -3648,12 +5956,12 @@
     <row r="28" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
       <c r="B28" s="8"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="16"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="15"/>
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
@@ -3693,12 +6001,12 @@
     <row r="29" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
       <c r="B29" s="8"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="16"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="15"/>
       <c r="I29"/>
       <c r="J29"/>
       <c r="K29"/>
@@ -3735,15 +6043,15 @@
       <c r="AP29"/>
       <c r="AQ29"/>
     </row>
-    <row r="30" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="10"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="18"/>
+    <row r="30" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="9"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="15"/>
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
@@ -3780,15 +6088,15 @@
       <c r="AP30"/>
       <c r="AQ30"/>
     </row>
-    <row r="31" spans="1:43" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
+    <row r="31" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="10"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="17"/>
       <c r="I31"/>
       <c r="J31"/>
       <c r="K31"/>
@@ -3825,7 +6133,51 @@
       <c r="AP31"/>
       <c r="AQ31"/>
     </row>
-    <row r="32" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:43" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32"/>
+      <c r="J32"/>
+      <c r="K32"/>
+      <c r="L32"/>
+      <c r="M32"/>
+      <c r="N32"/>
+      <c r="O32"/>
+      <c r="P32"/>
+      <c r="Q32"/>
+      <c r="R32"/>
+      <c r="S32"/>
+      <c r="T32"/>
+      <c r="U32"/>
+      <c r="V32"/>
+      <c r="W32"/>
+      <c r="X32"/>
+      <c r="Y32"/>
+      <c r="Z32"/>
+      <c r="AA32"/>
+      <c r="AB32"/>
+      <c r="AC32"/>
+      <c r="AD32"/>
+      <c r="AE32"/>
+      <c r="AF32"/>
+      <c r="AG32"/>
+      <c r="AH32"/>
+      <c r="AI32"/>
+      <c r="AJ32"/>
+      <c r="AK32"/>
+      <c r="AL32"/>
+      <c r="AM32"/>
+      <c r="AN32"/>
+      <c r="AO32"/>
+      <c r="AP32"/>
+      <c r="AQ32"/>
+    </row>
     <row r="33" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="34" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="35" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -3871,6 +6223,7 @@
     <row r="75" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="76" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="77" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="G1:H1"/>
@@ -3881,8 +6234,8 @@
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A24:H24"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
   </mergeCells>

</xml_diff>